<commit_message>
SDG&E 2026 WMP Workpapers and SCE covered conductor results
</commit_message>
<xml_diff>
--- a/WMP26/PGE/Mbar_PGE_Ign_CCvBare.xlsx
+++ b/WMP26/PGE/Mbar_PGE_Ign_CCvBare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwm/Work/WEEDS/Calculations/Workpapers/WMP26/PGE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC9B040-D023-1949-BC79-75C044E6AA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571D610C-DD36-0945-A8A5-96145CED0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{A4656C18-3F89-5247-B32C-A563D807BB58}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,7 +554,7 @@
         <v>154277811</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D5" si="0">C4/5280</f>
+        <f t="shared" ref="D4:D20" si="0">C4/5280</f>
         <v>29219.282386363637</v>
       </c>
       <c r="E4">
@@ -593,6 +593,17 @@
       <c r="B8">
         <v>58</v>
       </c>
+      <c r="C8">
+        <v>85018055</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>16101.904356060606</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E6:E20" si="2">B8/D8</f>
+        <v>3.6020584098283596E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -601,6 +612,17 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9">
+        <v>11977176</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2268.4045454545453</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>8.8167694955805953E-4</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -609,6 +631,17 @@
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="C10">
+        <v>3697017</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>700.1926136363636</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>1.4281784476511739E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -622,6 +655,17 @@
       <c r="B13">
         <v>23</v>
       </c>
+      <c r="C13">
+        <v>30827591</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>5838.5589015151518</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>3.9393282465697687E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -630,6 +674,17 @@
       <c r="B14">
         <v>0</v>
       </c>
+      <c r="C14">
+        <v>5324275</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1008.3854166666666</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -638,13 +693,24 @@
       <c r="B15">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>3416580</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>647.0795454545455</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -652,8 +718,20 @@
         <f>B8+B13</f>
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f>C8+C13</f>
+        <v>115845646</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>21940.463257575757</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>3.6918090128307455E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -661,14 +739,38 @@
         <f>B9+B14</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f>C9+C14</f>
+        <v>17301451</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3276.7899621212123</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>6.1035343220635079E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20">
         <f>B10+B15</f>
         <v>1</v>
+      </c>
+      <c r="C20">
+        <f>C10+C15</f>
+        <v>7113597</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1347.2721590909091</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>7.4224052894759148E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>